<commit_message>
Added test data for invalid login Created InvalidLogin
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="7752" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:P25"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,9 +21,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>akshara</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -339,15 +356,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>